<commit_message>
Updated code and added new tracks
</commit_message>
<xml_diff>
--- a/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
+++ b/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanshalgoyal/brown-formula-racing-sim/OpenLAP_matlab/vehicle_descriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE021B12-B5DD-BF4C-8168-068F46EDA95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0386DCF4-86EB-DE49-8D8D-F57C65A46AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1483,7 +1483,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="3">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -1856,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made small parameter edits
</commit_message>
<xml_diff>
--- a/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
+++ b/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanshalgoyal/brown-formula-racing-sim/OpenLAP_matlab/vehicle_descriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0386DCF4-86EB-DE49-8D8D-F57C65A46AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ACFCA5-E2B2-3041-A7A6-65444B535917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1437,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="3">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
@@ -1483,7 +1483,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="3">
-        <v>1.25</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
- Added auto2024 and endurance2024 - Cleaned up files
</commit_message>
<xml_diff>
--- a/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
+++ b/OpenLAP_matlab/vehicle_descriptions/Rhode Rage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanshalgoyal/brown-formula-racing-sim/OpenLAP_matlab/vehicle_descriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ACFCA5-E2B2-3041-A7A6-65444B535917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEFB7DB-25FC-4F49-B7C1-AC7777DEC2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1437,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="3">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
@@ -1483,7 +1483,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:G1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>